<commit_message>
Update state for test case
</commit_message>
<xml_diff>
--- a/Documentation/2. Casos de Prueba - Automatizacion API.xlsx
+++ b/Documentation/2. Casos de Prueba - Automatizacion API.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neoris0-my.sharepoint.com/personal/jhonny_ortega_neoris_com/Documents/Documentos/Computador Neoris Completo/Jhonny/Curso Udemy/Automatizacion/2. Pruebas Manuales/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EC5371G\OneDrive - NEORIS\Documentos\Computador Neoris Completo\Backend Automation\backend_karate\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="11_F25DC773A252ABDACC1048DEA9996F8E5BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53C33032-2D7E-491A-A457-9C3341BE3002}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B1FCE6-9920-4FF9-93DA-221731BE0097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="34995" windowHeight="19196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>DETALLE CASOS</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Usuarios</t>
-  </si>
-  <si>
-    <t>PENDIENTE</t>
   </si>
   <si>
     <t>Jhonny Aldair Ortega Ortega</t>
@@ -266,6 +263,12 @@
   </si>
   <si>
     <t>El codigo de respuesta para la solicitud debe ser 204</t>
+  </si>
+  <si>
+    <t>Exitoso</t>
+  </si>
+  <si>
+    <t>No Exitoso</t>
   </si>
 </sst>
 </file>
@@ -549,6 +552,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -567,10 +574,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -933,7 +936,7 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="M1" sqref="M1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -958,27 +961,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="26" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="28" t="s">
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="23" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1040,7 +1043,7 @@
         <v>45426</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>20</v>
@@ -1049,7 +1052,7 @@
         <v>21</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>22</v>
@@ -1058,22 +1061,22 @@
         <v>23</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J3" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="M3" s="13" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="N3" s="15"/>
       <c r="O3" s="14"/>
@@ -1085,16 +1088,16 @@
         <v>45426</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>22</v>
@@ -1103,22 +1106,22 @@
         <v>23</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="9" t="s">
+      <c r="L4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="9" t="s">
-        <v>36</v>
-      </c>
       <c r="M4" s="13" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="N4" s="15"/>
       <c r="O4" s="14"/>
@@ -1130,16 +1133,16 @@
         <v>45426</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>22</v>
@@ -1148,22 +1151,22 @@
         <v>23</v>
       </c>
       <c r="H5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="K5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>41</v>
-      </c>
       <c r="M5" s="13" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="N5" s="15"/>
       <c r="O5" s="14"/>
@@ -1175,16 +1178,16 @@
         <v>45426</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>22</v>
@@ -1193,22 +1196,22 @@
         <v>23</v>
       </c>
       <c r="H6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="J6" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="L6" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="M6" s="13" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="N6" s="15"/>
       <c r="O6" s="14"/>
@@ -1220,16 +1223,16 @@
         <v>45426</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>22</v>
@@ -1238,22 +1241,22 @@
         <v>23</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" s="9" t="s">
+      <c r="L7" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="L7" s="9" t="s">
-        <v>54</v>
-      </c>
       <c r="M7" s="13" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="N7" s="15"/>
       <c r="O7" s="14"/>
@@ -1265,16 +1268,16 @@
         <v>45426</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>22</v>
@@ -1283,22 +1286,22 @@
         <v>23</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M8" s="13" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="N8" s="15"/>
       <c r="O8" s="14"/>
@@ -1310,16 +1313,16 @@
         <v>45426</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>22</v>
@@ -1328,22 +1331,22 @@
         <v>23</v>
       </c>
       <c r="H9" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="J9" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="J9" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" s="9" t="s">
+      <c r="L9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="M9" s="13" t="s">
         <v>60</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>24</v>
       </c>
       <c r="N9" s="15"/>
       <c r="O9" s="14"/>

</xml_diff>

<commit_message>
changes file casos de prueba and add file colection
</commit_message>
<xml_diff>
--- a/Documentation/2. Casos de Prueba - Automatizacion API.xlsx
+++ b/Documentation/2. Casos de Prueba - Automatizacion API.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EC5371G\OneDrive - NEORIS\Documentos\Computador Neoris Completo\Backend Automation\backend_karate\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neoris0-my.sharepoint.com/personal/jhonny_ortega_neoris_com/Documents/Documentos/Computador Neoris Completo/Jhonny/Curso Udemy/Automatizacion/2. Pruebas Manuales/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B1FCE6-9920-4FF9-93DA-221731BE0097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="11_F25DC773A252ABDACC1048DEA9996F8E5BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6939A0B-1655-4F03-AC40-A6DA35665B78}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="34995" windowHeight="19196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ejecucion de Casos de Prueba" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
   <si>
     <t>DETALLE CASOS</t>
   </si>
   <si>
-    <t>EJECUCIÓN CORRIDA 1</t>
-  </si>
-  <si>
-    <t>EVIDENCIA</t>
-  </si>
-  <si>
     <t>Fecha Creación o Modificación del Caso</t>
   </si>
   <si>
@@ -72,19 +66,10 @@
     <t>Resultado Esperado</t>
   </si>
   <si>
-    <t>Estado C1</t>
-  </si>
-  <si>
     <t>ID Bug</t>
   </si>
   <si>
     <t>Comentario</t>
-  </si>
-  <si>
-    <t>Fecha Ejecución C1</t>
-  </si>
-  <si>
-    <t>Ruta y Nombre del Archivo</t>
   </si>
   <si>
     <t>Caso_01</t>
@@ -270,6 +255,21 @@
   <si>
     <t>No Exitoso</t>
   </si>
+  <si>
+    <t>EJECUCIÓN</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Fecha Ejecución</t>
+  </si>
+  <si>
+    <t>16 de mayo de 2024</t>
+  </si>
+  <si>
+    <t>Al enviar el campo "email" con el valor "prueba", sin comillas y sin que cumpla la estructura de un correo, el usuario se crea de forma exitosa, lo cual NO es correcto</t>
+  </si>
 </sst>
 </file>
 
@@ -279,7 +279,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-C0A]d\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,6 +350,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -383,7 +390,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -398,17 +405,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -465,7 +461,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -503,21 +499,13 @@
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -540,7 +528,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -549,10 +537,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="3" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -573,6 +557,13 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -933,425 +924,433 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:P1"/>
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="14.375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="9" style="12"/>
-    <col min="4" max="4" width="8.875" style="12" customWidth="1"/>
-    <col min="5" max="5" width="18.625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="12.75" style="12" customWidth="1"/>
-    <col min="7" max="7" width="14.625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="12" style="12" customWidth="1"/>
-    <col min="9" max="9" width="15.25" style="12" customWidth="1"/>
-    <col min="10" max="10" width="20.375" style="12" customWidth="1"/>
-    <col min="11" max="11" width="32.625" style="12" customWidth="1"/>
-    <col min="12" max="12" width="21.375" style="12" customWidth="1"/>
-    <col min="13" max="13" width="16.125" style="12" customWidth="1"/>
-    <col min="14" max="14" width="9.625" style="12" customWidth="1"/>
-    <col min="15" max="15" width="12.5" style="12" customWidth="1"/>
-    <col min="16" max="16" width="13.75" style="12" customWidth="1"/>
-    <col min="17" max="17" width="16.375" style="12" customWidth="1"/>
+    <col min="1" max="1" width="16.875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="14.375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="9" style="10"/>
+    <col min="4" max="4" width="8.875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="18.625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="12.75" style="10" customWidth="1"/>
+    <col min="7" max="7" width="14.625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="12" style="10" customWidth="1"/>
+    <col min="9" max="9" width="15.25" style="10" customWidth="1"/>
+    <col min="10" max="10" width="20.375" style="10" customWidth="1"/>
+    <col min="11" max="11" width="32.625" style="10" customWidth="1"/>
+    <col min="12" max="12" width="21.375" style="10" customWidth="1"/>
+    <col min="13" max="13" width="16.125" style="10" customWidth="1"/>
+    <col min="14" max="14" width="9.625" style="10" customWidth="1"/>
+    <col min="15" max="15" width="12.5" style="10" customWidth="1"/>
+    <col min="16" max="16" width="13.75" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="27" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+    </row>
+    <row r="2" spans="1:16" s="10" customFormat="1" ht="40.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="23" t="s">
+      <c r="B2" s="16" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" s="12" customFormat="1" ht="40.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="P2" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q2" s="19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="285.3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="285.3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45426</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="F3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="K3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="N3" s="13"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="N3" s="15"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="11"/>
     </row>
-    <row r="4" spans="1:17" ht="135.85" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="135.85" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45426</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>34</v>
-      </c>
       <c r="L4" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="13"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="N4" s="15"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="11"/>
     </row>
-    <row r="5" spans="1:17" ht="156.9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="156.9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45426</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="9" t="s">
-        <v>44</v>
-      </c>
       <c r="L5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" s="13"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="N5" s="15"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="11"/>
     </row>
-    <row r="6" spans="1:17" ht="156.9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="217.4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45426</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="M6" s="13" t="s">
+      <c r="M6" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="N6" s="26">
+        <v>1</v>
+      </c>
+      <c r="O6" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="N6" s="15"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="11"/>
+      <c r="P6" s="27" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" ht="142.65" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="142.65" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45426</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>52</v>
-      </c>
       <c r="L7" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="M7" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="N7" s="13"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="N7" s="15"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="11"/>
     </row>
-    <row r="8" spans="1:17" ht="156.9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="217.4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45426</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>34</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="M8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="N8" s="26">
+        <v>2</v>
+      </c>
+      <c r="O8" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="N8" s="15"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="11"/>
+      <c r="P8" s="27" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="9" spans="1:17" ht="135.85" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="135.85" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45426</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="M9" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="M9" s="13" t="s">
+      <c r="N9" s="13"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="N9" s="15"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>